<commit_message>
GLUE QNLI Processor for run_classifier
Added QNLI to run_classifier.py so it can process SQuAD train and dev sets.  However, the tsv files from GLUE do not have original qid to match up predictions between QA and Classifier.

So, TODO: save a pickled copy of train_features from run_squad for both train and dev.  Load those files into run_classifier.py, so both models are trained on the exact same data.  Line 1329 in run_squad.

Also, fixed unicode error in run_squad logging.
</commit_message>
<xml_diff>
--- a/examples/output/190304-02_46-errors-DEV.xlsx
+++ b/examples/output/190304-02_46-errors-DEV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klalande/Box Sync/klalande/Kevin/Online Courses/2017 Stanford Graduate Certificate/CS224/02_Project/01_Code/pytorch-pretrained-BERT/examples/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54EF6DC4-2CFD-9748-9A99-9782A853EDF5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2DA4D4-961F-B64F-9508-0062A0F3AB8F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10160" yWindow="3240" windowWidth="25980" windowHeight="23860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>gold_file</t>
   </si>
@@ -147,6 +147,24 @@
   </si>
   <si>
     <t>Length of Answer</t>
+  </si>
+  <si>
+    <t>03/12/2019 00:52:05 - INFO - __main__ -   ***** Read Squad Examples *****</t>
+  </si>
+  <si>
+    <t>03/12/2019 00:52:05 - INFO - __main__ -     Num Squad examples = 130319</t>
+  </si>
+  <si>
+    <t>03/12/2019 00:52:05 - INFO - __main__ -     Num Squad examples with No Answer = 43498</t>
+  </si>
+  <si>
+    <t>03/12/2019 06:19:01 - INFO - __main__ -   ***** Read Squad Examples *****</t>
+  </si>
+  <si>
+    <t>03/12/2019 06:19:01 - INFO - __main__ -     Num Squad examples = 62062</t>
+  </si>
+  <si>
+    <t>03/12/2019 06:19:01 - INFO - __main__ -     Num Squad examples with No Answer = 14099</t>
   </si>
 </sst>
 </file>
@@ -567,14 +585,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:AC467"/>
+  <dimension ref="C2:AC467"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="2" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="3" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -582,6 +605,9 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
@@ -590,6 +616,9 @@
       <c r="D4">
         <v>6078</v>
       </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
@@ -606,6 +635,9 @@
       <c r="D6">
         <v>6078</v>
       </c>
+      <c r="K6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
@@ -613,6 +645,9 @@
       </c>
       <c r="D7">
         <v>74.695623560381705</v>
+      </c>
+      <c r="K7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:29" x14ac:dyDescent="0.2">
@@ -621,6 +656,9 @@
       </c>
       <c r="D8">
         <v>77.345931680068418</v>
+      </c>
+      <c r="K8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="3:29" x14ac:dyDescent="0.2">
@@ -1310,7 +1348,7 @@
         <v>3726</v>
       </c>
       <c r="H24" s="3">
-        <f>G24/$G$44</f>
+        <f t="shared" ref="H24:H43" si="0">G24/$G$44</f>
         <v>0.59086584205518555</v>
       </c>
       <c r="K24" s="1">
@@ -1376,7 +1414,7 @@
         <v>714</v>
       </c>
       <c r="H25" s="3">
-        <f>G25/$G$44</f>
+        <f t="shared" si="0"/>
         <v>0.11322549952426261</v>
       </c>
       <c r="K25" s="1">
@@ -1442,7 +1480,7 @@
         <v>605</v>
       </c>
       <c r="H26" s="3">
-        <f>G26/$G$44</f>
+        <f t="shared" si="0"/>
         <v>9.594037424674913E-2</v>
       </c>
       <c r="K26" s="1">
@@ -1508,7 +1546,7 @@
         <v>561</v>
       </c>
       <c r="H27" s="3">
-        <f>G27/$G$44</f>
+        <f t="shared" si="0"/>
         <v>8.8962892483349196E-2</v>
       </c>
       <c r="K27" s="1">
@@ -1574,7 +1612,7 @@
         <v>275</v>
       </c>
       <c r="H28" s="3">
-        <f>G28/$G$44</f>
+        <f t="shared" si="0"/>
         <v>4.3609261021249603E-2</v>
       </c>
       <c r="K28" s="1">
@@ -1640,7 +1678,7 @@
         <v>274</v>
       </c>
       <c r="H29" s="3">
-        <f>G29/$G$44</f>
+        <f t="shared" si="0"/>
         <v>4.3450681890263243E-2</v>
       </c>
       <c r="K29" s="1">
@@ -1706,7 +1744,7 @@
         <v>92</v>
       </c>
       <c r="H30" s="3">
-        <f>G30/$G$44</f>
+        <f t="shared" si="0"/>
         <v>1.4589280050745322E-2</v>
       </c>
       <c r="K30" s="1">
@@ -1772,7 +1810,7 @@
         <v>14</v>
       </c>
       <c r="H31" s="3">
-        <f>G31/$G$44</f>
+        <f t="shared" si="0"/>
         <v>2.2201078338090706E-3</v>
       </c>
       <c r="K31" s="1">
@@ -1838,7 +1876,7 @@
         <v>9</v>
       </c>
       <c r="H32" s="3">
-        <f>G32/$G$44</f>
+        <f t="shared" si="0"/>
         <v>1.4272121788772598E-3</v>
       </c>
       <c r="K32" s="1">
@@ -1904,7 +1942,7 @@
         <v>7</v>
       </c>
       <c r="H33" s="3">
-        <f>G33/$G$44</f>
+        <f t="shared" si="0"/>
         <v>1.1100539169045353E-3</v>
       </c>
       <c r="K33" s="1">
@@ -1970,7 +2008,7 @@
         <v>7</v>
       </c>
       <c r="H34" s="3">
-        <f>G34/$G$44</f>
+        <f t="shared" si="0"/>
         <v>1.1100539169045353E-3</v>
       </c>
       <c r="K34" s="1">
@@ -2036,7 +2074,7 @@
         <v>7</v>
       </c>
       <c r="H35" s="3">
-        <f>G35/$G$44</f>
+        <f t="shared" si="0"/>
         <v>1.1100539169045353E-3</v>
       </c>
       <c r="K35" s="1">
@@ -2102,7 +2140,7 @@
         <v>6</v>
       </c>
       <c r="H36" s="3">
-        <f>G36/$G$44</f>
+        <f t="shared" si="0"/>
         <v>9.5147478591817321E-4</v>
       </c>
       <c r="K36" s="1">
@@ -2168,7 +2206,7 @@
         <v>2</v>
       </c>
       <c r="H37" s="3">
-        <f>G37/$G$44</f>
+        <f t="shared" si="0"/>
         <v>3.1715826197272439E-4</v>
       </c>
       <c r="K37" s="1">
@@ -2234,7 +2272,7 @@
         <v>2</v>
       </c>
       <c r="H38" s="3">
-        <f>G38/$G$44</f>
+        <f t="shared" si="0"/>
         <v>3.1715826197272439E-4</v>
       </c>
       <c r="K38" s="1">
@@ -2300,7 +2338,7 @@
         <v>1</v>
       </c>
       <c r="H39" s="3">
-        <f>G39/$G$44</f>
+        <f t="shared" si="0"/>
         <v>1.5857913098636219E-4</v>
       </c>
       <c r="K39" s="1">
@@ -2366,7 +2404,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="3">
-        <f>G40/$G$44</f>
+        <f t="shared" si="0"/>
         <v>1.5857913098636219E-4</v>
       </c>
       <c r="K40" s="1">
@@ -2432,7 +2470,7 @@
         <v>1</v>
       </c>
       <c r="H41" s="3">
-        <f>G41/$G$44</f>
+        <f t="shared" si="0"/>
         <v>1.5857913098636219E-4</v>
       </c>
       <c r="K41" s="1">
@@ -2498,7 +2536,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="3">
-        <f>G42/$G$44</f>
+        <f t="shared" si="0"/>
         <v>1.5857913098636219E-4</v>
       </c>
       <c r="K42" s="1">
@@ -2564,7 +2602,7 @@
         <v>1</v>
       </c>
       <c r="H43" s="3">
-        <f>G43/$G$44</f>
+        <f t="shared" si="0"/>
         <v>1.5857913098636219E-4</v>
       </c>
       <c r="K43" s="1">
@@ -2776,15 +2814,15 @@
         <v>what</v>
       </c>
       <c r="D47" s="3">
-        <f>D24/$G24</f>
+        <f t="shared" ref="D47:F53" si="1">D24/$G24</f>
         <v>0.20531400966183574</v>
       </c>
       <c r="E47" s="3">
-        <f>E24/$G24</f>
+        <f t="shared" si="1"/>
         <v>0.75201288244766507</v>
       </c>
       <c r="F47" s="3">
-        <f>F24/$G24</f>
+        <f t="shared" si="1"/>
         <v>4.2673107890499197E-2</v>
       </c>
       <c r="H47" s="4">
@@ -2839,23 +2877,23 @@
     </row>
     <row r="48" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C48" t="str">
-        <f t="shared" ref="C48:C53" si="0">C25</f>
+        <f t="shared" ref="C48:C53" si="2">C25</f>
         <v>who</v>
       </c>
       <c r="D48" s="3">
-        <f>D25/$G25</f>
+        <f t="shared" si="1"/>
         <v>0.20448179271708683</v>
       </c>
       <c r="E48" s="3">
-        <f>E25/$G25</f>
+        <f t="shared" si="1"/>
         <v>0.76050420168067223</v>
       </c>
       <c r="F48" s="3">
-        <f>F25/$G25</f>
+        <f t="shared" si="1"/>
         <v>3.5014005602240897E-2</v>
       </c>
       <c r="H48" s="4">
-        <f t="shared" ref="H48:H53" si="1">H25</f>
+        <f t="shared" ref="H48:H53" si="3">H25</f>
         <v>0.11322549952426261</v>
       </c>
       <c r="K48" s="1">
@@ -2906,23 +2944,23 @@
     </row>
     <row r="49" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>how</v>
       </c>
       <c r="D49" s="3">
-        <f>D26/$G26</f>
+        <f t="shared" si="1"/>
         <v>0.22975206611570248</v>
       </c>
       <c r="E49" s="3">
-        <f>E26/$G26</f>
+        <f t="shared" si="1"/>
         <v>0.71074380165289253</v>
       </c>
       <c r="F49" s="3">
-        <f>F26/$G26</f>
+        <f t="shared" si="1"/>
         <v>5.9504132231404959E-2</v>
       </c>
       <c r="H49" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.594037424674913E-2</v>
       </c>
       <c r="K49" s="1">
@@ -2973,23 +3011,23 @@
     </row>
     <row r="50" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>when</v>
       </c>
       <c r="D50" s="3">
-        <f>D27/$G27</f>
+        <f t="shared" si="1"/>
         <v>0.20142602495543671</v>
       </c>
       <c r="E50" s="3">
-        <f>E27/$G27</f>
+        <f t="shared" si="1"/>
         <v>0.77718360071301251</v>
       </c>
       <c r="F50" s="3">
-        <f>F27/$G27</f>
+        <f t="shared" si="1"/>
         <v>2.1390374331550801E-2</v>
       </c>
       <c r="H50" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.8962892483349196E-2</v>
       </c>
       <c r="K50" s="1">
@@ -3040,23 +3078,23 @@
     </row>
     <row r="51" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>where</v>
       </c>
       <c r="D51" s="3">
-        <f>D28/$G28</f>
+        <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
       <c r="E51" s="3">
-        <f>E28/$G28</f>
+        <f t="shared" si="1"/>
         <v>0.72</v>
       </c>
       <c r="F51" s="3">
-        <f>F28/$G28</f>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="H51" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.3609261021249603E-2</v>
       </c>
       <c r="K51" s="1">
@@ -3107,23 +3145,23 @@
     </row>
     <row r="52" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>which</v>
       </c>
       <c r="D52" s="3">
-        <f>D29/$G29</f>
+        <f t="shared" si="1"/>
         <v>0.22992700729927007</v>
       </c>
       <c r="E52" s="3">
-        <f>E29/$G29</f>
+        <f t="shared" si="1"/>
         <v>0.73722627737226276</v>
       </c>
       <c r="F52" s="3">
-        <f>F29/$G29</f>
+        <f t="shared" si="1"/>
         <v>3.2846715328467155E-2</v>
       </c>
       <c r="H52" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.3450681890263243E-2</v>
       </c>
       <c r="K52" s="1">
@@ -3174,23 +3212,23 @@
     </row>
     <row r="53" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>why</v>
       </c>
       <c r="D53" s="3">
-        <f>D30/$G30</f>
+        <f t="shared" si="1"/>
         <v>0.2391304347826087</v>
       </c>
       <c r="E53" s="3">
-        <f>E30/$G30</f>
+        <f t="shared" si="1"/>
         <v>0.58695652173913049</v>
       </c>
       <c r="F53" s="3">
-        <f>F30/$G30</f>
+        <f t="shared" si="1"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="H53" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.4589280050745322E-2</v>
       </c>
       <c r="K53" s="1">

</xml_diff>

<commit_message>
Split data into train/val, Log train/val loss
load_split_data(args, data, split=0.9)
- new function to split train data into train and validation

New CLI parameters
--log_traindev_loss
--val_steps

Added tensorboard_api

Added ensemble

Added map_location to load_state_dict to allow GPU-trained models to be loaded on CPU

Added pickle dump of eval_examples, eval_features, all_results for debug analysis
</commit_message>
<xml_diff>
--- a/examples/output/190304-02_46-errors-DEV.xlsx
+++ b/examples/output/190304-02_46-errors-DEV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klalande/Box Sync/klalande/Kevin/Online Courses/2017 Stanford Graduate Certificate/CS224/02_Project/01_Code/pytorch-pretrained-BERT/examples/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2DA4D4-961F-B64F-9508-0062A0F3AB8F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133DDF9C-3A03-4F4E-9B02-B1B80CC3050E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10160" yWindow="3240" windowWidth="25980" windowHeight="23860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26520" yWindow="4420" windowWidth="24000" windowHeight="23860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="errorAnalysis" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>gold_file</t>
   </si>
@@ -165,6 +165,36 @@
   </si>
   <si>
     <t>03/12/2019 06:19:01 - INFO - __main__ -     Num Squad examples with No Answer = 14099</t>
+  </si>
+  <si>
+    <t>03/14/2019 04:42:10 - INFO - __main__ -   ***** Read Squad Examples *****</t>
+  </si>
+  <si>
+    <t>03/14/2019 04:42:10 - INFO - __main__ -     Num Squad examples = 75335</t>
+  </si>
+  <si>
+    <t>03/14/2019 04:42:10 - INFO - __main__ -     Num Squad examples with No Answer = 20644</t>
+  </si>
+  <si>
+    <t>03/14/2019 05:14:52 - INFO - __main__ -     Saving train features into cached file /home/klalande/squad/data/train-v2.0.json_bert-base-uncased_True_False_384_128_64</t>
+  </si>
+  <si>
+    <t>03/14/2019 05:15:48 - INFO - __main__ -   ***** Running training *****</t>
+  </si>
+  <si>
+    <t>03/14/2019 05:15:48 - INFO - __main__ -     Num orig examples = 205653</t>
+  </si>
+  <si>
+    <t>03/14/2019 05:15:48 - INFO - __main__ -     Num split examples = 459272</t>
+  </si>
+  <si>
+    <t>03/14/2019 05:15:48 - INFO - __main__ -     Batch size = 32</t>
+  </si>
+  <si>
+    <t>03/14/2019 05:15:48 - INFO - __main__ -     Num steps = 12852</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -587,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:AC467"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2:AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -597,6 +627,9 @@
       <c r="K2" t="s">
         <v>40</v>
       </c>
+      <c r="AC2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
@@ -608,6 +641,9 @@
       <c r="K3" t="s">
         <v>41</v>
       </c>
+      <c r="AC3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
@@ -619,6 +655,9 @@
       <c r="K4" t="s">
         <v>42</v>
       </c>
+      <c r="AC4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="5" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
@@ -627,6 +666,9 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
+      <c r="AC5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="6" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
@@ -638,6 +680,12 @@
       <c r="K6" t="s">
         <v>43</v>
       </c>
+      <c r="T6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
@@ -648,6 +696,12 @@
       </c>
       <c r="K7" t="s">
         <v>44</v>
+      </c>
+      <c r="T7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="3:29" x14ac:dyDescent="0.2">
@@ -659,6 +713,12 @@
       </c>
       <c r="K8" t="s">
         <v>45</v>
+      </c>
+      <c r="T8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="3:29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Correct scaling of train loss vs val loss; fixed map_location for torch.load GPU to CPU mapping
</commit_message>
<xml_diff>
--- a/examples/output/190304-02_46-errors-DEV.xlsx
+++ b/examples/output/190304-02_46-errors-DEV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klalande/Box Sync/klalande/Kevin/Online Courses/2017 Stanford Graduate Certificate/CS224/02_Project/01_Code/pytorch-pretrained-BERT/examples/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133DDF9C-3A03-4F4E-9B02-B1B80CC3050E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24D708B-D1C3-EB43-AA25-06E44C0B2FFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26520" yWindow="4420" windowWidth="24000" windowHeight="23860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15680" yWindow="1300" windowWidth="29300" windowHeight="23860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="errorAnalysis" sheetId="1" r:id="rId1"/>
@@ -268,7 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -276,6 +276,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:AC467"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2:AC8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13:X156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -843,6 +844,14 @@
       <c r="V13">
         <v>1</v>
       </c>
+      <c r="W13" s="5">
+        <f>V13</f>
+        <v>1</v>
+      </c>
+      <c r="X13" s="3">
+        <f>W13/$V$157</f>
+        <v>1.6452780519907864E-4</v>
+      </c>
       <c r="Y13" s="1">
         <v>0</v>
       </c>
@@ -908,6 +917,14 @@
       </c>
       <c r="V14">
         <v>3</v>
+      </c>
+      <c r="W14" s="5">
+        <f>V14+W13</f>
+        <v>4</v>
+      </c>
+      <c r="X14" s="3">
+        <f t="shared" ref="X14:X77" si="0">W14/$V$157</f>
+        <v>6.5811122079631457E-4</v>
       </c>
       <c r="Y14" s="1">
         <v>1</v>
@@ -972,6 +989,14 @@
       <c r="V15">
         <v>3</v>
       </c>
+      <c r="W15" s="5">
+        <f t="shared" ref="W15:W78" si="1">V15+W14</f>
+        <v>7</v>
+      </c>
+      <c r="X15" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1516946363935505E-3</v>
+      </c>
       <c r="Y15" s="1">
         <v>2</v>
       </c>
@@ -1031,6 +1056,14 @@
       <c r="V16">
         <v>3</v>
       </c>
+      <c r="W16" s="5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="X16" s="3">
+        <f t="shared" si="0"/>
+        <v>1.6452780519907865E-3</v>
+      </c>
       <c r="Y16" s="1">
         <v>3</v>
       </c>
@@ -1078,6 +1111,14 @@
       <c r="V17">
         <v>4</v>
       </c>
+      <c r="W17" s="5">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="X17" s="3">
+        <f t="shared" si="0"/>
+        <v>2.3033892727871009E-3</v>
+      </c>
       <c r="Y17" s="1">
         <v>4</v>
       </c>
@@ -1125,6 +1166,14 @@
       <c r="V18">
         <v>3</v>
       </c>
+      <c r="W18" s="5">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="X18" s="3">
+        <f t="shared" si="0"/>
+        <v>2.7969726883843369E-3</v>
+      </c>
       <c r="Y18" s="1">
         <v>5</v>
       </c>
@@ -1172,6 +1221,14 @@
       <c r="V19">
         <v>5</v>
       </c>
+      <c r="W19" s="5">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="X19" s="3">
+        <f t="shared" si="0"/>
+        <v>3.6196117143797303E-3</v>
+      </c>
       <c r="Y19" s="1">
         <v>6</v>
       </c>
@@ -1219,6 +1276,14 @@
       <c r="V20">
         <v>13</v>
       </c>
+      <c r="W20" s="5">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="X20" s="3">
+        <f t="shared" si="0"/>
+        <v>5.7584731819677526E-3</v>
+      </c>
       <c r="Y20" s="1">
         <v>7</v>
       </c>
@@ -1266,6 +1331,14 @@
       <c r="V21">
         <v>11</v>
       </c>
+      <c r="W21" s="5">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="X21" s="3">
+        <f t="shared" si="0"/>
+        <v>7.5682790391576179E-3</v>
+      </c>
       <c r="Y21" s="1">
         <v>8</v>
       </c>
@@ -1316,6 +1389,14 @@
       <c r="V22">
         <v>10</v>
       </c>
+      <c r="W22" s="5">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="X22" s="3">
+        <f t="shared" si="0"/>
+        <v>9.2135570911484038E-3</v>
+      </c>
       <c r="Y22" s="1">
         <v>9</v>
       </c>
@@ -1374,6 +1455,14 @@
       </c>
       <c r="V23">
         <v>19</v>
+      </c>
+      <c r="W23" s="5">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="X23" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2339585389930898E-2</v>
       </c>
       <c r="Y23" s="1">
         <v>10</v>
@@ -1408,7 +1497,7 @@
         <v>3726</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" ref="H24:H43" si="0">G24/$G$44</f>
+        <f t="shared" ref="H24:H43" si="2">G24/$G$44</f>
         <v>0.59086584205518555</v>
       </c>
       <c r="K24" s="1">
@@ -1440,6 +1529,14 @@
       </c>
       <c r="V24">
         <v>27</v>
+      </c>
+      <c r="W24" s="5">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="X24" s="3">
+        <f t="shared" si="0"/>
+        <v>1.6781836130306021E-2</v>
       </c>
       <c r="Y24" s="1">
         <v>11</v>
@@ -1474,7 +1571,7 @@
         <v>714</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11322549952426261</v>
       </c>
       <c r="K25" s="1">
@@ -1506,6 +1603,14 @@
       </c>
       <c r="V25">
         <v>21</v>
+      </c>
+      <c r="W25" s="5">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="X25" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0236920039486673E-2</v>
       </c>
       <c r="Y25" s="1">
         <v>12</v>
@@ -1540,7 +1645,7 @@
         <v>605</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.594037424674913E-2</v>
       </c>
       <c r="K26" s="1">
@@ -1572,6 +1677,14 @@
       </c>
       <c r="V26">
         <v>18</v>
+      </c>
+      <c r="W26" s="5">
+        <f t="shared" si="1"/>
+        <v>141</v>
+      </c>
+      <c r="X26" s="3">
+        <f t="shared" si="0"/>
+        <v>2.3198420533070089E-2</v>
       </c>
       <c r="Y26" s="1">
         <v>13</v>
@@ -1606,7 +1719,7 @@
         <v>561</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.8962892483349196E-2</v>
       </c>
       <c r="K27" s="1">
@@ -1638,6 +1751,14 @@
       </c>
       <c r="V27">
         <v>31</v>
+      </c>
+      <c r="W27" s="5">
+        <f t="shared" si="1"/>
+        <v>172</v>
+      </c>
+      <c r="X27" s="3">
+        <f t="shared" si="0"/>
+        <v>2.8298782494241528E-2</v>
       </c>
       <c r="Y27" s="1">
         <v>14</v>
@@ -1672,7 +1793,7 @@
         <v>275</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.3609261021249603E-2</v>
       </c>
       <c r="K28" s="1">
@@ -1704,6 +1825,14 @@
       </c>
       <c r="V28">
         <v>27</v>
+      </c>
+      <c r="W28" s="5">
+        <f t="shared" si="1"/>
+        <v>199</v>
+      </c>
+      <c r="X28" s="3">
+        <f t="shared" si="0"/>
+        <v>3.2741033234616648E-2</v>
       </c>
       <c r="Y28" s="1">
         <v>15</v>
@@ -1738,7 +1867,7 @@
         <v>274</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.3450681890263243E-2</v>
       </c>
       <c r="K29" s="1">
@@ -1770,6 +1899,14 @@
       </c>
       <c r="V29">
         <v>40</v>
+      </c>
+      <c r="W29" s="5">
+        <f t="shared" si="1"/>
+        <v>239</v>
+      </c>
+      <c r="X29" s="3">
+        <f t="shared" si="0"/>
+        <v>3.9322145442579795E-2</v>
       </c>
       <c r="Y29" s="1">
         <v>16</v>
@@ -1804,7 +1941,7 @@
         <v>92</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.4589280050745322E-2</v>
       </c>
       <c r="K30" s="1">
@@ -1836,6 +1973,14 @@
       </c>
       <c r="V30">
         <v>55</v>
+      </c>
+      <c r="W30" s="5">
+        <f t="shared" si="1"/>
+        <v>294</v>
+      </c>
+      <c r="X30" s="3">
+        <f t="shared" si="0"/>
+        <v>4.8371174728529122E-2</v>
       </c>
       <c r="Y30" s="1">
         <v>17</v>
@@ -1870,7 +2015,7 @@
         <v>14</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.2201078338090706E-3</v>
       </c>
       <c r="K31" s="1">
@@ -1902,6 +2047,14 @@
       </c>
       <c r="V31">
         <v>58</v>
+      </c>
+      <c r="W31" s="5">
+        <f t="shared" si="1"/>
+        <v>352</v>
+      </c>
+      <c r="X31" s="3">
+        <f t="shared" si="0"/>
+        <v>5.7913787430075685E-2</v>
       </c>
       <c r="Y31" s="1">
         <v>18</v>
@@ -1936,7 +2089,7 @@
         <v>9</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.4272121788772598E-3</v>
       </c>
       <c r="K32" s="1">
@@ -1968,6 +2121,14 @@
       </c>
       <c r="V32">
         <v>57</v>
+      </c>
+      <c r="W32" s="5">
+        <f t="shared" si="1"/>
+        <v>409</v>
+      </c>
+      <c r="X32" s="3">
+        <f t="shared" si="0"/>
+        <v>6.7291872326423169E-2</v>
       </c>
       <c r="Y32" s="1">
         <v>19</v>
@@ -2002,7 +2163,7 @@
         <v>7</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1100539169045353E-3</v>
       </c>
       <c r="K33" s="1">
@@ -2034,6 +2195,14 @@
       </c>
       <c r="V33">
         <v>51</v>
+      </c>
+      <c r="W33" s="5">
+        <f t="shared" si="1"/>
+        <v>460</v>
+      </c>
+      <c r="X33" s="3">
+        <f t="shared" si="0"/>
+        <v>7.5682790391576174E-2</v>
       </c>
       <c r="Y33" s="1">
         <v>20</v>
@@ -2068,7 +2237,7 @@
         <v>7</v>
       </c>
       <c r="H34" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1100539169045353E-3</v>
       </c>
       <c r="K34" s="1">
@@ -2100,6 +2269,14 @@
       </c>
       <c r="V34">
         <v>67</v>
+      </c>
+      <c r="W34" s="5">
+        <f t="shared" si="1"/>
+        <v>527</v>
+      </c>
+      <c r="X34" s="3">
+        <f t="shared" si="0"/>
+        <v>8.6706153339914452E-2</v>
       </c>
       <c r="Y34" s="1">
         <v>21</v>
@@ -2134,7 +2311,7 @@
         <v>7</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1100539169045353E-3</v>
       </c>
       <c r="K35" s="1">
@@ -2166,6 +2343,14 @@
       </c>
       <c r="V35">
         <v>89</v>
+      </c>
+      <c r="W35" s="5">
+        <f t="shared" si="1"/>
+        <v>616</v>
+      </c>
+      <c r="X35" s="3">
+        <f t="shared" si="0"/>
+        <v>0.10134912800263245</v>
       </c>
       <c r="Y35" s="1">
         <v>22</v>
@@ -2200,7 +2385,7 @@
         <v>6</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.5147478591817321E-4</v>
       </c>
       <c r="K36" s="1">
@@ -2232,6 +2417,14 @@
       </c>
       <c r="V36">
         <v>79</v>
+      </c>
+      <c r="W36" s="5">
+        <f t="shared" si="1"/>
+        <v>695</v>
+      </c>
+      <c r="X36" s="3">
+        <f t="shared" si="0"/>
+        <v>0.11434682461335965</v>
       </c>
       <c r="Y36" s="1">
         <v>23</v>
@@ -2266,7 +2459,7 @@
         <v>2</v>
       </c>
       <c r="H37" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1715826197272439E-4</v>
       </c>
       <c r="K37" s="1">
@@ -2298,6 +2491,14 @@
       </c>
       <c r="V37">
         <v>92</v>
+      </c>
+      <c r="W37" s="5">
+        <f t="shared" si="1"/>
+        <v>787</v>
+      </c>
+      <c r="X37" s="3">
+        <f t="shared" si="0"/>
+        <v>0.12948338269167489</v>
       </c>
       <c r="Y37" s="1">
         <v>24</v>
@@ -2332,7 +2533,7 @@
         <v>2</v>
       </c>
       <c r="H38" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.1715826197272439E-4</v>
       </c>
       <c r="K38" s="1">
@@ -2364,6 +2565,14 @@
       </c>
       <c r="V38">
         <v>101</v>
+      </c>
+      <c r="W38" s="5">
+        <f t="shared" si="1"/>
+        <v>888</v>
+      </c>
+      <c r="X38" s="3">
+        <f t="shared" si="0"/>
+        <v>0.14610069101678183</v>
       </c>
       <c r="Y38" s="1">
         <v>25</v>
@@ -2398,7 +2607,7 @@
         <v>1</v>
       </c>
       <c r="H39" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.5857913098636219E-4</v>
       </c>
       <c r="K39" s="1">
@@ -2430,6 +2639,14 @@
       </c>
       <c r="V39">
         <v>95</v>
+      </c>
+      <c r="W39" s="5">
+        <f t="shared" si="1"/>
+        <v>983</v>
+      </c>
+      <c r="X39" s="3">
+        <f t="shared" si="0"/>
+        <v>0.16173083251069431</v>
       </c>
       <c r="Y39" s="1">
         <v>26</v>
@@ -2464,7 +2681,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.5857913098636219E-4</v>
       </c>
       <c r="K40" s="1">
@@ -2496,6 +2713,14 @@
       </c>
       <c r="V40">
         <v>102</v>
+      </c>
+      <c r="W40" s="5">
+        <f t="shared" si="1"/>
+        <v>1085</v>
+      </c>
+      <c r="X40" s="3">
+        <f t="shared" si="0"/>
+        <v>0.17851266864100032</v>
       </c>
       <c r="Y40" s="1">
         <v>27</v>
@@ -2530,7 +2755,7 @@
         <v>1</v>
       </c>
       <c r="H41" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.5857913098636219E-4</v>
       </c>
       <c r="K41" s="1">
@@ -2562,6 +2787,14 @@
       </c>
       <c r="V41">
         <v>117</v>
+      </c>
+      <c r="W41" s="5">
+        <f t="shared" si="1"/>
+        <v>1202</v>
+      </c>
+      <c r="X41" s="3">
+        <f t="shared" si="0"/>
+        <v>0.19776242184929252</v>
       </c>
       <c r="Y41" s="1">
         <v>28</v>
@@ -2596,7 +2829,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.5857913098636219E-4</v>
       </c>
       <c r="K42" s="1">
@@ -2628,6 +2861,14 @@
       </c>
       <c r="V42">
         <v>112</v>
+      </c>
+      <c r="W42" s="5">
+        <f t="shared" si="1"/>
+        <v>1314</v>
+      </c>
+      <c r="X42" s="3">
+        <f t="shared" si="0"/>
+        <v>0.21618953603158933</v>
       </c>
       <c r="Y42" s="1">
         <v>29</v>
@@ -2662,7 +2903,7 @@
         <v>1</v>
       </c>
       <c r="H43" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.5857913098636219E-4</v>
       </c>
       <c r="K43" s="1">
@@ -2694,6 +2935,14 @@
       </c>
       <c r="V43">
         <v>134</v>
+      </c>
+      <c r="W43" s="5">
+        <f t="shared" si="1"/>
+        <v>1448</v>
+      </c>
+      <c r="X43" s="3">
+        <f t="shared" si="0"/>
+        <v>0.23823626192826589</v>
       </c>
       <c r="Y43" s="1">
         <v>30</v>
@@ -2758,6 +3007,14 @@
       <c r="V44">
         <v>139</v>
       </c>
+      <c r="W44" s="5">
+        <f t="shared" si="1"/>
+        <v>1587</v>
+      </c>
+      <c r="X44" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2611056268509378</v>
+      </c>
       <c r="Y44" s="1">
         <v>31</v>
       </c>
@@ -2805,6 +3062,14 @@
       <c r="V45">
         <v>132</v>
       </c>
+      <c r="W45" s="5">
+        <f t="shared" si="1"/>
+        <v>1719</v>
+      </c>
+      <c r="X45" s="3">
+        <f t="shared" si="0"/>
+        <v>0.28282329713721621</v>
+      </c>
       <c r="Y45" s="1">
         <v>32</v>
       </c>
@@ -2851,6 +3116,14 @@
       </c>
       <c r="V46">
         <v>147</v>
+      </c>
+      <c r="W46" s="5">
+        <f t="shared" si="1"/>
+        <v>1866</v>
+      </c>
+      <c r="X46" s="3">
+        <f t="shared" si="0"/>
+        <v>0.30700888450148073</v>
       </c>
       <c r="Y46" s="1">
         <v>33</v>
@@ -2874,15 +3147,15 @@
         <v>what</v>
       </c>
       <c r="D47" s="3">
-        <f t="shared" ref="D47:F53" si="1">D24/$G24</f>
+        <f t="shared" ref="D47:F53" si="3">D24/$G24</f>
         <v>0.20531400966183574</v>
       </c>
       <c r="E47" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.75201288244766507</v>
       </c>
       <c r="F47" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.2673107890499197E-2</v>
       </c>
       <c r="H47" s="4">
@@ -2919,6 +3192,14 @@
       <c r="V47">
         <v>107</v>
       </c>
+      <c r="W47" s="5">
+        <f t="shared" si="1"/>
+        <v>1973</v>
+      </c>
+      <c r="X47" s="3">
+        <f t="shared" si="0"/>
+        <v>0.32461335965778215</v>
+      </c>
       <c r="Y47" s="1">
         <v>34</v>
       </c>
@@ -2937,23 +3218,23 @@
     </row>
     <row r="48" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C48" t="str">
-        <f t="shared" ref="C48:C53" si="2">C25</f>
+        <f t="shared" ref="C48:C53" si="4">C25</f>
         <v>who</v>
       </c>
       <c r="D48" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.20448179271708683</v>
       </c>
       <c r="E48" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.76050420168067223</v>
       </c>
       <c r="F48" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.5014005602240897E-2</v>
       </c>
       <c r="H48" s="4">
-        <f t="shared" ref="H48:H53" si="3">H25</f>
+        <f t="shared" ref="H48:H53" si="5">H25</f>
         <v>0.11322549952426261</v>
       </c>
       <c r="K48" s="1">
@@ -2986,6 +3267,14 @@
       <c r="V48">
         <v>132</v>
       </c>
+      <c r="W48" s="5">
+        <f t="shared" si="1"/>
+        <v>2105</v>
+      </c>
+      <c r="X48" s="3">
+        <f t="shared" si="0"/>
+        <v>0.34633102994406056</v>
+      </c>
       <c r="Y48" s="1">
         <v>35</v>
       </c>
@@ -3004,23 +3293,23 @@
     </row>
     <row r="49" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C49" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>how</v>
       </c>
       <c r="D49" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.22975206611570248</v>
       </c>
       <c r="E49" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.71074380165289253</v>
       </c>
       <c r="F49" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.9504132231404959E-2</v>
       </c>
       <c r="H49" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.594037424674913E-2</v>
       </c>
       <c r="K49" s="1">
@@ -3053,6 +3342,14 @@
       <c r="V49">
         <v>101</v>
       </c>
+      <c r="W49" s="5">
+        <f t="shared" si="1"/>
+        <v>2206</v>
+      </c>
+      <c r="X49" s="3">
+        <f t="shared" si="0"/>
+        <v>0.3629483382691675</v>
+      </c>
       <c r="Y49" s="1">
         <v>36</v>
       </c>
@@ -3071,23 +3368,23 @@
     </row>
     <row r="50" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>when</v>
       </c>
       <c r="D50" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.20142602495543671</v>
       </c>
       <c r="E50" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.77718360071301251</v>
       </c>
       <c r="F50" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.1390374331550801E-2</v>
       </c>
       <c r="H50" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.8962892483349196E-2</v>
       </c>
       <c r="K50" s="1">
@@ -3120,6 +3417,14 @@
       <c r="V50">
         <v>118</v>
       </c>
+      <c r="W50" s="5">
+        <f t="shared" si="1"/>
+        <v>2324</v>
+      </c>
+      <c r="X50" s="3">
+        <f t="shared" si="0"/>
+        <v>0.38236261928265874</v>
+      </c>
       <c r="Y50" s="1">
         <v>37</v>
       </c>
@@ -3138,23 +3443,23 @@
     </row>
     <row r="51" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C51" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>where</v>
       </c>
       <c r="D51" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.24</v>
       </c>
       <c r="E51" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.72</v>
       </c>
       <c r="F51" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
       <c r="H51" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.3609261021249603E-2</v>
       </c>
       <c r="K51" s="1">
@@ -3187,6 +3492,14 @@
       <c r="V51">
         <v>126</v>
       </c>
+      <c r="W51" s="5">
+        <f t="shared" si="1"/>
+        <v>2450</v>
+      </c>
+      <c r="X51" s="3">
+        <f t="shared" si="0"/>
+        <v>0.40309312273774267</v>
+      </c>
       <c r="Y51" s="1">
         <v>38</v>
       </c>
@@ -3205,23 +3518,23 @@
     </row>
     <row r="52" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C52" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>which</v>
       </c>
       <c r="D52" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.22992700729927007</v>
       </c>
       <c r="E52" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.73722627737226276</v>
       </c>
       <c r="F52" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.2846715328467155E-2</v>
       </c>
       <c r="H52" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.3450681890263243E-2</v>
       </c>
       <c r="K52" s="1">
@@ -3254,6 +3567,14 @@
       <c r="V52">
         <v>134</v>
       </c>
+      <c r="W52" s="5">
+        <f t="shared" si="1"/>
+        <v>2584</v>
+      </c>
+      <c r="X52" s="3">
+        <f t="shared" si="0"/>
+        <v>0.42513984863441923</v>
+      </c>
       <c r="Y52" s="1">
         <v>39</v>
       </c>
@@ -3272,23 +3593,23 @@
     </row>
     <row r="53" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C53" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>why</v>
       </c>
       <c r="D53" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.2391304347826087</v>
       </c>
       <c r="E53" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.58695652173913049</v>
       </c>
       <c r="F53" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="H53" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.4589280050745322E-2</v>
       </c>
       <c r="K53" s="1">
@@ -3320,6 +3641,14 @@
       </c>
       <c r="V53">
         <v>122</v>
+      </c>
+      <c r="W53" s="5">
+        <f t="shared" si="1"/>
+        <v>2706</v>
+      </c>
+      <c r="X53" s="3">
+        <f t="shared" si="0"/>
+        <v>0.44521224086870681</v>
       </c>
       <c r="Y53" s="1">
         <v>40</v>
@@ -3371,6 +3700,14 @@
       <c r="V54">
         <v>139</v>
       </c>
+      <c r="W54" s="5">
+        <f t="shared" si="1"/>
+        <v>2845</v>
+      </c>
+      <c r="X54" s="3">
+        <f t="shared" si="0"/>
+        <v>0.46808160579137875</v>
+      </c>
       <c r="Y54" s="1">
         <v>41</v>
       </c>
@@ -3418,6 +3755,14 @@
       <c r="V55">
         <v>131</v>
       </c>
+      <c r="W55" s="5">
+        <f t="shared" si="1"/>
+        <v>2976</v>
+      </c>
+      <c r="X55" s="3">
+        <f t="shared" si="0"/>
+        <v>0.48963474827245806</v>
+      </c>
       <c r="Y55" s="1">
         <v>42</v>
       </c>
@@ -3465,6 +3810,14 @@
       <c r="V56">
         <v>125</v>
       </c>
+      <c r="W56" s="5">
+        <f t="shared" si="1"/>
+        <v>3101</v>
+      </c>
+      <c r="X56" s="3">
+        <f t="shared" si="0"/>
+        <v>0.51020072392234284</v>
+      </c>
       <c r="Y56" s="1">
         <v>43</v>
       </c>
@@ -3512,6 +3865,14 @@
       <c r="V57">
         <v>128</v>
       </c>
+      <c r="W57" s="5">
+        <f t="shared" si="1"/>
+        <v>3229</v>
+      </c>
+      <c r="X57" s="3">
+        <f t="shared" si="0"/>
+        <v>0.53126028298782491</v>
+      </c>
       <c r="Y57" s="1">
         <v>44</v>
       </c>
@@ -3559,6 +3920,14 @@
       <c r="V58">
         <v>128</v>
       </c>
+      <c r="W58" s="5">
+        <f t="shared" si="1"/>
+        <v>3357</v>
+      </c>
+      <c r="X58" s="3">
+        <f t="shared" si="0"/>
+        <v>0.55231984205330698</v>
+      </c>
       <c r="Y58" s="1">
         <v>45</v>
       </c>
@@ -3606,6 +3975,14 @@
       <c r="V59">
         <v>151</v>
       </c>
+      <c r="W59" s="5">
+        <f t="shared" si="1"/>
+        <v>3508</v>
+      </c>
+      <c r="X59" s="3">
+        <f t="shared" si="0"/>
+        <v>0.57716354063836783</v>
+      </c>
       <c r="Y59" s="1">
         <v>46</v>
       </c>
@@ -3653,6 +4030,14 @@
       <c r="V60">
         <v>129</v>
       </c>
+      <c r="W60" s="5">
+        <f t="shared" si="1"/>
+        <v>3637</v>
+      </c>
+      <c r="X60" s="3">
+        <f t="shared" si="0"/>
+        <v>0.59838762750904906</v>
+      </c>
       <c r="Y60" s="1">
         <v>47</v>
       </c>
@@ -3700,6 +4085,14 @@
       <c r="V61">
         <v>113</v>
       </c>
+      <c r="W61" s="5">
+        <f t="shared" si="1"/>
+        <v>3750</v>
+      </c>
+      <c r="X61" s="3">
+        <f t="shared" si="0"/>
+        <v>0.61697926949654491</v>
+      </c>
       <c r="Y61" s="1">
         <v>48</v>
       </c>
@@ -3747,6 +4140,14 @@
       <c r="V62">
         <v>115</v>
       </c>
+      <c r="W62" s="5">
+        <f t="shared" si="1"/>
+        <v>3865</v>
+      </c>
+      <c r="X62" s="3">
+        <f t="shared" si="0"/>
+        <v>0.63589996709443897</v>
+      </c>
       <c r="Y62" s="1">
         <v>49</v>
       </c>
@@ -3794,6 +4195,14 @@
       <c r="V63">
         <v>96</v>
       </c>
+      <c r="W63" s="5">
+        <f t="shared" si="1"/>
+        <v>3961</v>
+      </c>
+      <c r="X63" s="3">
+        <f t="shared" si="0"/>
+        <v>0.65169463639355052</v>
+      </c>
       <c r="Y63" s="1">
         <v>50</v>
       </c>
@@ -3841,6 +4250,14 @@
       <c r="V64">
         <v>108</v>
       </c>
+      <c r="W64" s="5">
+        <f t="shared" si="1"/>
+        <v>4069</v>
+      </c>
+      <c r="X64" s="3">
+        <f t="shared" si="0"/>
+        <v>0.66946363935505104</v>
+      </c>
       <c r="Y64" s="1">
         <v>51</v>
       </c>
@@ -3888,6 +4305,14 @@
       <c r="V65">
         <v>97</v>
       </c>
+      <c r="W65" s="5">
+        <f t="shared" si="1"/>
+        <v>4166</v>
+      </c>
+      <c r="X65" s="3">
+        <f t="shared" si="0"/>
+        <v>0.68542283645936164</v>
+      </c>
       <c r="Y65" s="1">
         <v>52</v>
       </c>
@@ -3935,6 +4360,14 @@
       <c r="V66">
         <v>88</v>
       </c>
+      <c r="W66" s="5">
+        <f t="shared" si="1"/>
+        <v>4254</v>
+      </c>
+      <c r="X66" s="3">
+        <f t="shared" si="0"/>
+        <v>0.69990128331688051</v>
+      </c>
       <c r="Y66" s="1">
         <v>53</v>
       </c>
@@ -3982,6 +4415,14 @@
       <c r="V67">
         <v>100</v>
       </c>
+      <c r="W67" s="5">
+        <f t="shared" si="1"/>
+        <v>4354</v>
+      </c>
+      <c r="X67" s="3">
+        <f t="shared" si="0"/>
+        <v>0.71635406383678846</v>
+      </c>
       <c r="Y67" s="1">
         <v>54</v>
       </c>
@@ -4029,6 +4470,14 @@
       <c r="V68">
         <v>67</v>
       </c>
+      <c r="W68" s="5">
+        <f t="shared" si="1"/>
+        <v>4421</v>
+      </c>
+      <c r="X68" s="3">
+        <f t="shared" si="0"/>
+        <v>0.72737742678512673</v>
+      </c>
       <c r="Y68" s="1">
         <v>55</v>
       </c>
@@ -4076,6 +4525,14 @@
       <c r="V69">
         <v>70</v>
       </c>
+      <c r="W69" s="5">
+        <f t="shared" si="1"/>
+        <v>4491</v>
+      </c>
+      <c r="X69" s="3">
+        <f t="shared" si="0"/>
+        <v>0.73889437314906214</v>
+      </c>
       <c r="Y69" s="1">
         <v>56</v>
       </c>
@@ -4123,6 +4580,14 @@
       <c r="V70">
         <v>84</v>
       </c>
+      <c r="W70" s="5">
+        <f t="shared" si="1"/>
+        <v>4575</v>
+      </c>
+      <c r="X70" s="3">
+        <f t="shared" si="0"/>
+        <v>0.75271470878578484</v>
+      </c>
       <c r="Y70" s="1">
         <v>57</v>
       </c>
@@ -4170,6 +4635,14 @@
       <c r="V71">
         <v>65</v>
       </c>
+      <c r="W71" s="5">
+        <f t="shared" si="1"/>
+        <v>4640</v>
+      </c>
+      <c r="X71" s="3">
+        <f t="shared" si="0"/>
+        <v>0.76340901612372492</v>
+      </c>
       <c r="Y71" s="1">
         <v>58</v>
       </c>
@@ -4217,6 +4690,14 @@
       <c r="V72">
         <v>63</v>
       </c>
+      <c r="W72" s="5">
+        <f t="shared" si="1"/>
+        <v>4703</v>
+      </c>
+      <c r="X72" s="3">
+        <f t="shared" si="0"/>
+        <v>0.77377426785126691</v>
+      </c>
       <c r="Y72" s="1">
         <v>59</v>
       </c>
@@ -4264,6 +4745,14 @@
       <c r="V73">
         <v>57</v>
       </c>
+      <c r="W73" s="5">
+        <f t="shared" si="1"/>
+        <v>4760</v>
+      </c>
+      <c r="X73" s="3">
+        <f t="shared" si="0"/>
+        <v>0.7831523527476143</v>
+      </c>
       <c r="Y73" s="1">
         <v>60</v>
       </c>
@@ -4311,6 +4800,14 @@
       <c r="V74">
         <v>60</v>
       </c>
+      <c r="W74" s="5">
+        <f t="shared" si="1"/>
+        <v>4820</v>
+      </c>
+      <c r="X74" s="3">
+        <f t="shared" si="0"/>
+        <v>0.79302402105955905</v>
+      </c>
       <c r="Y74" s="1">
         <v>61</v>
       </c>
@@ -4358,6 +4855,14 @@
       <c r="V75">
         <v>69</v>
       </c>
+      <c r="W75" s="5">
+        <f t="shared" si="1"/>
+        <v>4889</v>
+      </c>
+      <c r="X75" s="3">
+        <f t="shared" si="0"/>
+        <v>0.80437643961829552</v>
+      </c>
       <c r="Y75" s="1">
         <v>62</v>
       </c>
@@ -4405,6 +4910,14 @@
       <c r="V76">
         <v>53</v>
       </c>
+      <c r="W76" s="5">
+        <f t="shared" si="1"/>
+        <v>4942</v>
+      </c>
+      <c r="X76" s="3">
+        <f t="shared" si="0"/>
+        <v>0.81309641329384663</v>
+      </c>
       <c r="Y76" s="1">
         <v>63</v>
       </c>
@@ -4452,6 +4965,14 @@
       <c r="V77">
         <v>56</v>
       </c>
+      <c r="W77" s="5">
+        <f t="shared" si="1"/>
+        <v>4998</v>
+      </c>
+      <c r="X77" s="3">
+        <f t="shared" si="0"/>
+        <v>0.82230997038499509</v>
+      </c>
       <c r="Y77" s="1">
         <v>64</v>
       </c>
@@ -4499,6 +5020,14 @@
       <c r="V78">
         <v>65</v>
       </c>
+      <c r="W78" s="5">
+        <f t="shared" si="1"/>
+        <v>5063</v>
+      </c>
+      <c r="X78" s="3">
+        <f t="shared" ref="X78:X141" si="6">W78/$V$157</f>
+        <v>0.83300427772293517</v>
+      </c>
       <c r="Y78" s="1">
         <v>65</v>
       </c>
@@ -4546,6 +5075,14 @@
       <c r="V79">
         <v>60</v>
       </c>
+      <c r="W79" s="5">
+        <f t="shared" ref="W79:W142" si="7">V79+W78</f>
+        <v>5123</v>
+      </c>
+      <c r="X79" s="3">
+        <f t="shared" si="6"/>
+        <v>0.84287594603487992</v>
+      </c>
       <c r="Y79" s="1">
         <v>66</v>
       </c>
@@ -4593,6 +5130,14 @@
       <c r="V80">
         <v>50</v>
       </c>
+      <c r="W80" s="5">
+        <f t="shared" si="7"/>
+        <v>5173</v>
+      </c>
+      <c r="X80" s="3">
+        <f t="shared" si="6"/>
+        <v>0.85110233629483378</v>
+      </c>
       <c r="Y80" s="1">
         <v>67</v>
       </c>
@@ -4640,6 +5185,14 @@
       <c r="V81">
         <v>39</v>
       </c>
+      <c r="W81" s="5">
+        <f t="shared" si="7"/>
+        <v>5212</v>
+      </c>
+      <c r="X81" s="3">
+        <f t="shared" si="6"/>
+        <v>0.85751892069759794</v>
+      </c>
       <c r="Y81" s="1">
         <v>68</v>
       </c>
@@ -4687,6 +5240,14 @@
       <c r="V82">
         <v>45</v>
       </c>
+      <c r="W82" s="5">
+        <f t="shared" si="7"/>
+        <v>5257</v>
+      </c>
+      <c r="X82" s="3">
+        <f t="shared" si="6"/>
+        <v>0.86492267193155647</v>
+      </c>
       <c r="Y82" s="1">
         <v>69</v>
       </c>
@@ -4734,6 +5295,14 @@
       <c r="V83">
         <v>43</v>
       </c>
+      <c r="W83" s="5">
+        <f t="shared" si="7"/>
+        <v>5300</v>
+      </c>
+      <c r="X83" s="3">
+        <f t="shared" si="6"/>
+        <v>0.87199736755511681</v>
+      </c>
       <c r="Y83" s="1">
         <v>70</v>
       </c>
@@ -4781,6 +5350,14 @@
       <c r="V84">
         <v>40</v>
       </c>
+      <c r="W84" s="5">
+        <f t="shared" si="7"/>
+        <v>5340</v>
+      </c>
+      <c r="X84" s="3">
+        <f t="shared" si="6"/>
+        <v>0.87857847976308001</v>
+      </c>
       <c r="Y84" s="1">
         <v>71</v>
       </c>
@@ -4828,6 +5405,14 @@
       <c r="V85">
         <v>38</v>
       </c>
+      <c r="W85" s="5">
+        <f t="shared" si="7"/>
+        <v>5378</v>
+      </c>
+      <c r="X85" s="3">
+        <f t="shared" si="6"/>
+        <v>0.8848305363606449</v>
+      </c>
       <c r="Y85" s="1">
         <v>72</v>
       </c>
@@ -4875,6 +5460,14 @@
       <c r="V86">
         <v>40</v>
       </c>
+      <c r="W86" s="5">
+        <f t="shared" si="7"/>
+        <v>5418</v>
+      </c>
+      <c r="X86" s="3">
+        <f t="shared" si="6"/>
+        <v>0.89141164856860811</v>
+      </c>
       <c r="Y86" s="1">
         <v>73</v>
       </c>
@@ -4922,6 +5515,14 @@
       <c r="V87">
         <v>38</v>
       </c>
+      <c r="W87" s="5">
+        <f t="shared" si="7"/>
+        <v>5456</v>
+      </c>
+      <c r="X87" s="3">
+        <f t="shared" si="6"/>
+        <v>0.89766370516617311</v>
+      </c>
       <c r="Y87" s="1">
         <v>74</v>
       </c>
@@ -4969,6 +5570,14 @@
       <c r="V88">
         <v>33</v>
       </c>
+      <c r="W88" s="5">
+        <f t="shared" si="7"/>
+        <v>5489</v>
+      </c>
+      <c r="X88" s="3">
+        <f t="shared" si="6"/>
+        <v>0.90309312273774267</v>
+      </c>
       <c r="Y88" s="1">
         <v>75</v>
       </c>
@@ -5016,6 +5625,14 @@
       <c r="V89">
         <v>46</v>
       </c>
+      <c r="W89" s="5">
+        <f t="shared" si="7"/>
+        <v>5535</v>
+      </c>
+      <c r="X89" s="3">
+        <f t="shared" si="6"/>
+        <v>0.91066140177690025</v>
+      </c>
       <c r="Y89" s="1">
         <v>76</v>
       </c>
@@ -5063,6 +5680,14 @@
       <c r="V90">
         <v>40</v>
       </c>
+      <c r="W90" s="5">
+        <f t="shared" si="7"/>
+        <v>5575</v>
+      </c>
+      <c r="X90" s="3">
+        <f t="shared" si="6"/>
+        <v>0.91724251398486345</v>
+      </c>
       <c r="Y90" s="1">
         <v>77</v>
       </c>
@@ -5110,6 +5735,14 @@
       <c r="V91">
         <v>28</v>
       </c>
+      <c r="W91" s="5">
+        <f t="shared" si="7"/>
+        <v>5603</v>
+      </c>
+      <c r="X91" s="3">
+        <f t="shared" si="6"/>
+        <v>0.92184929253043768</v>
+      </c>
       <c r="Y91" s="1">
         <v>78</v>
       </c>
@@ -5157,6 +5790,14 @@
       <c r="V92">
         <v>31</v>
       </c>
+      <c r="W92" s="5">
+        <f t="shared" si="7"/>
+        <v>5634</v>
+      </c>
+      <c r="X92" s="3">
+        <f t="shared" si="6"/>
+        <v>0.92694965449160904</v>
+      </c>
       <c r="Y92" s="1">
         <v>79</v>
       </c>
@@ -5204,6 +5845,14 @@
       <c r="V93">
         <v>22</v>
       </c>
+      <c r="W93" s="5">
+        <f t="shared" si="7"/>
+        <v>5656</v>
+      </c>
+      <c r="X93" s="3">
+        <f t="shared" si="6"/>
+        <v>0.93056926620598879</v>
+      </c>
       <c r="Y93" s="1">
         <v>80</v>
       </c>
@@ -5251,6 +5900,14 @@
       <c r="V94">
         <v>27</v>
       </c>
+      <c r="W94" s="5">
+        <f t="shared" si="7"/>
+        <v>5683</v>
+      </c>
+      <c r="X94" s="3">
+        <f t="shared" si="6"/>
+        <v>0.93501151694636397</v>
+      </c>
       <c r="Y94" s="1">
         <v>81</v>
       </c>
@@ -5298,6 +5955,14 @@
       <c r="V95">
         <v>28</v>
       </c>
+      <c r="W95" s="5">
+        <f t="shared" si="7"/>
+        <v>5711</v>
+      </c>
+      <c r="X95" s="3">
+        <f t="shared" si="6"/>
+        <v>0.93961829549193809</v>
+      </c>
       <c r="Y95" s="1">
         <v>82</v>
       </c>
@@ -5345,6 +6010,14 @@
       <c r="V96">
         <v>26</v>
       </c>
+      <c r="W96" s="5">
+        <f t="shared" si="7"/>
+        <v>5737</v>
+      </c>
+      <c r="X96" s="3">
+        <f t="shared" si="6"/>
+        <v>0.94389601842711424</v>
+      </c>
       <c r="Y96" s="1">
         <v>83</v>
       </c>
@@ -5392,6 +6065,14 @@
       <c r="V97">
         <v>28</v>
       </c>
+      <c r="W97" s="5">
+        <f t="shared" si="7"/>
+        <v>5765</v>
+      </c>
+      <c r="X97" s="3">
+        <f t="shared" si="6"/>
+        <v>0.94850279697268836</v>
+      </c>
       <c r="Y97" s="1">
         <v>84</v>
       </c>
@@ -5439,6 +6120,14 @@
       <c r="V98">
         <v>17</v>
       </c>
+      <c r="W98" s="5">
+        <f t="shared" si="7"/>
+        <v>5782</v>
+      </c>
+      <c r="X98" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95129976966107277</v>
+      </c>
       <c r="Y98" s="1">
         <v>85</v>
       </c>
@@ -5486,6 +6175,14 @@
       <c r="V99">
         <v>21</v>
       </c>
+      <c r="W99" s="5">
+        <f t="shared" si="7"/>
+        <v>5803</v>
+      </c>
+      <c r="X99" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95475485357025336</v>
+      </c>
       <c r="Y99" s="1">
         <v>86</v>
       </c>
@@ -5533,6 +6230,14 @@
       <c r="V100">
         <v>15</v>
       </c>
+      <c r="W100" s="5">
+        <f t="shared" si="7"/>
+        <v>5818</v>
+      </c>
+      <c r="X100" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95722277064823957</v>
+      </c>
       <c r="Y100" s="1">
         <v>87</v>
       </c>
@@ -5580,6 +6285,14 @@
       <c r="V101">
         <v>19</v>
       </c>
+      <c r="W101" s="5">
+        <f t="shared" si="7"/>
+        <v>5837</v>
+      </c>
+      <c r="X101" s="3">
+        <f t="shared" si="6"/>
+        <v>0.96034879894702208</v>
+      </c>
       <c r="Y101" s="1">
         <v>88</v>
       </c>
@@ -5627,6 +6340,14 @@
       <c r="V102">
         <v>9</v>
       </c>
+      <c r="W102" s="5">
+        <f t="shared" si="7"/>
+        <v>5846</v>
+      </c>
+      <c r="X102" s="3">
+        <f t="shared" si="6"/>
+        <v>0.9618295491938138</v>
+      </c>
       <c r="Y102" s="1">
         <v>89</v>
       </c>
@@ -5674,6 +6395,14 @@
       <c r="V103">
         <v>14</v>
       </c>
+      <c r="W103" s="5">
+        <f t="shared" si="7"/>
+        <v>5860</v>
+      </c>
+      <c r="X103" s="3">
+        <f t="shared" si="6"/>
+        <v>0.96413293846660086</v>
+      </c>
       <c r="Y103" s="1">
         <v>90</v>
       </c>
@@ -5721,6 +6450,14 @@
       <c r="V104">
         <v>18</v>
       </c>
+      <c r="W104" s="5">
+        <f t="shared" si="7"/>
+        <v>5878</v>
+      </c>
+      <c r="X104" s="3">
+        <f t="shared" si="6"/>
+        <v>0.96709443896018432</v>
+      </c>
       <c r="Y104" s="1">
         <v>92</v>
       </c>
@@ -5768,6 +6505,14 @@
       <c r="V105">
         <v>9</v>
       </c>
+      <c r="W105" s="5">
+        <f t="shared" si="7"/>
+        <v>5887</v>
+      </c>
+      <c r="X105" s="3">
+        <f t="shared" si="6"/>
+        <v>0.96857518920697594</v>
+      </c>
       <c r="Y105" s="1">
         <v>94</v>
       </c>
@@ -5815,6 +6560,14 @@
       <c r="V106">
         <v>7</v>
       </c>
+      <c r="W106" s="5">
+        <f t="shared" si="7"/>
+        <v>5894</v>
+      </c>
+      <c r="X106" s="3">
+        <f t="shared" si="6"/>
+        <v>0.96972688384336958</v>
+      </c>
       <c r="Y106" s="1">
         <v>96</v>
       </c>
@@ -5862,6 +6615,14 @@
       <c r="V107">
         <v>8</v>
       </c>
+      <c r="W107" s="5">
+        <f t="shared" si="7"/>
+        <v>5902</v>
+      </c>
+      <c r="X107" s="3">
+        <f t="shared" si="6"/>
+        <v>0.97104310628496215</v>
+      </c>
       <c r="Y107" s="1">
         <v>98</v>
       </c>
@@ -5909,6 +6670,14 @@
       <c r="V108">
         <v>12</v>
       </c>
+      <c r="W108" s="5">
+        <f t="shared" si="7"/>
+        <v>5914</v>
+      </c>
+      <c r="X108" s="3">
+        <f t="shared" si="6"/>
+        <v>0.97301743994735113</v>
+      </c>
       <c r="Y108" s="1">
         <v>99</v>
       </c>
@@ -5956,6 +6725,14 @@
       <c r="V109">
         <v>9</v>
       </c>
+      <c r="W109" s="5">
+        <f t="shared" si="7"/>
+        <v>5923</v>
+      </c>
+      <c r="X109" s="3">
+        <f t="shared" si="6"/>
+        <v>0.97449819019414285</v>
+      </c>
       <c r="Y109" s="1">
         <v>100</v>
       </c>
@@ -6003,6 +6780,14 @@
       <c r="V110">
         <v>6</v>
       </c>
+      <c r="W110" s="5">
+        <f t="shared" si="7"/>
+        <v>5929</v>
+      </c>
+      <c r="X110" s="3">
+        <f t="shared" si="6"/>
+        <v>0.97548535702533723</v>
+      </c>
       <c r="Y110" s="1">
         <v>102</v>
       </c>
@@ -6050,6 +6835,14 @@
       <c r="V111">
         <v>9</v>
       </c>
+      <c r="W111" s="5">
+        <f t="shared" si="7"/>
+        <v>5938</v>
+      </c>
+      <c r="X111" s="3">
+        <f t="shared" si="6"/>
+        <v>0.97696610727212896</v>
+      </c>
       <c r="Y111" s="1">
         <v>104</v>
       </c>
@@ -6097,6 +6890,14 @@
       <c r="V112">
         <v>7</v>
       </c>
+      <c r="W112" s="5">
+        <f t="shared" si="7"/>
+        <v>5945</v>
+      </c>
+      <c r="X112" s="3">
+        <f t="shared" si="6"/>
+        <v>0.97811780190852249</v>
+      </c>
       <c r="Y112" s="1">
         <v>105</v>
       </c>
@@ -6144,6 +6945,14 @@
       <c r="V113">
         <v>6</v>
       </c>
+      <c r="W113" s="5">
+        <f t="shared" si="7"/>
+        <v>5951</v>
+      </c>
+      <c r="X113" s="3">
+        <f t="shared" si="6"/>
+        <v>0.97910496873971697</v>
+      </c>
       <c r="Y113" s="1">
         <v>107</v>
       </c>
@@ -6191,6 +7000,14 @@
       <c r="V114">
         <v>5</v>
       </c>
+      <c r="W114" s="5">
+        <f t="shared" si="7"/>
+        <v>5956</v>
+      </c>
+      <c r="X114" s="3">
+        <f t="shared" si="6"/>
+        <v>0.97992760776571242</v>
+      </c>
       <c r="Y114" s="1">
         <v>109</v>
       </c>
@@ -6238,6 +7055,14 @@
       <c r="V115">
         <v>4</v>
       </c>
+      <c r="W115" s="5">
+        <f t="shared" si="7"/>
+        <v>5960</v>
+      </c>
+      <c r="X115" s="3">
+        <f t="shared" si="6"/>
+        <v>0.9805857189865087</v>
+      </c>
       <c r="Y115" s="1">
         <v>111</v>
       </c>
@@ -6285,6 +7110,14 @@
       <c r="V116">
         <v>7</v>
       </c>
+      <c r="W116" s="5">
+        <f t="shared" si="7"/>
+        <v>5967</v>
+      </c>
+      <c r="X116" s="3">
+        <f t="shared" si="6"/>
+        <v>0.98173741362290223</v>
+      </c>
       <c r="Y116" s="1">
         <v>113</v>
       </c>
@@ -6332,6 +7165,14 @@
       <c r="V117">
         <v>4</v>
       </c>
+      <c r="W117" s="5">
+        <f t="shared" si="7"/>
+        <v>5971</v>
+      </c>
+      <c r="X117" s="3">
+        <f t="shared" si="6"/>
+        <v>0.98239552484369863</v>
+      </c>
       <c r="Y117" s="1">
         <v>114</v>
       </c>
@@ -6379,6 +7220,14 @@
       <c r="V118">
         <v>5</v>
       </c>
+      <c r="W118" s="5">
+        <f t="shared" si="7"/>
+        <v>5976</v>
+      </c>
+      <c r="X118" s="3">
+        <f t="shared" si="6"/>
+        <v>0.98321816386969396</v>
+      </c>
       <c r="Y118" s="1">
         <v>118</v>
       </c>
@@ -6426,6 +7275,14 @@
       <c r="V119">
         <v>7</v>
       </c>
+      <c r="W119" s="5">
+        <f t="shared" si="7"/>
+        <v>5983</v>
+      </c>
+      <c r="X119" s="3">
+        <f t="shared" si="6"/>
+        <v>0.98436985850608749</v>
+      </c>
       <c r="Y119" s="1">
         <v>121</v>
       </c>
@@ -6473,6 +7330,14 @@
       <c r="V120">
         <v>7</v>
       </c>
+      <c r="W120" s="5">
+        <f t="shared" si="7"/>
+        <v>5990</v>
+      </c>
+      <c r="X120" s="3">
+        <f t="shared" si="6"/>
+        <v>0.98552155314248113</v>
+      </c>
       <c r="Y120" s="1">
         <v>124</v>
       </c>
@@ -6520,6 +7385,14 @@
       <c r="V121">
         <v>6</v>
       </c>
+      <c r="W121" s="5">
+        <f t="shared" si="7"/>
+        <v>5996</v>
+      </c>
+      <c r="X121" s="3">
+        <f t="shared" si="6"/>
+        <v>0.98650871997367551</v>
+      </c>
       <c r="Y121" s="1">
         <v>126</v>
       </c>
@@ -6567,6 +7440,14 @@
       <c r="V122">
         <v>2</v>
       </c>
+      <c r="W122" s="5">
+        <f t="shared" si="7"/>
+        <v>5998</v>
+      </c>
+      <c r="X122" s="3">
+        <f t="shared" si="6"/>
+        <v>0.98683777558407371</v>
+      </c>
       <c r="Y122" s="1">
         <v>128</v>
       </c>
@@ -6614,6 +7495,14 @@
       <c r="V123">
         <v>6</v>
       </c>
+      <c r="W123" s="5">
+        <f t="shared" si="7"/>
+        <v>6004</v>
+      </c>
+      <c r="X123" s="3">
+        <f t="shared" si="6"/>
+        <v>0.98782494241526819</v>
+      </c>
       <c r="Y123" s="1">
         <v>134</v>
       </c>
@@ -6661,6 +7550,14 @@
       <c r="V124">
         <v>4</v>
       </c>
+      <c r="W124" s="5">
+        <f t="shared" si="7"/>
+        <v>6008</v>
+      </c>
+      <c r="X124" s="3">
+        <f t="shared" si="6"/>
+        <v>0.98848305363606448</v>
+      </c>
       <c r="Y124" s="1">
         <v>139</v>
       </c>
@@ -6708,6 +7605,14 @@
       <c r="V125">
         <v>5</v>
       </c>
+      <c r="W125" s="5">
+        <f t="shared" si="7"/>
+        <v>6013</v>
+      </c>
+      <c r="X125" s="3">
+        <f t="shared" si="6"/>
+        <v>0.98930569266205992</v>
+      </c>
       <c r="Y125" s="1">
         <v>140</v>
       </c>
@@ -6755,6 +7660,14 @@
       <c r="V126">
         <v>4</v>
       </c>
+      <c r="W126" s="5">
+        <f t="shared" si="7"/>
+        <v>6017</v>
+      </c>
+      <c r="X126" s="3">
+        <f t="shared" si="6"/>
+        <v>0.98996380388285621</v>
+      </c>
       <c r="Y126" s="1">
         <v>141</v>
       </c>
@@ -6802,6 +7715,14 @@
       <c r="V127">
         <v>6</v>
       </c>
+      <c r="W127" s="5">
+        <f t="shared" si="7"/>
+        <v>6023</v>
+      </c>
+      <c r="X127" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99095097071405069</v>
+      </c>
       <c r="Y127" s="1">
         <v>143</v>
       </c>
@@ -6849,6 +7770,14 @@
       <c r="V128">
         <v>3</v>
       </c>
+      <c r="W128" s="5">
+        <f t="shared" si="7"/>
+        <v>6026</v>
+      </c>
+      <c r="X128" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99144455412964794</v>
+      </c>
       <c r="Y128" s="1">
         <v>144</v>
       </c>
@@ -6896,6 +7825,14 @@
       <c r="V129">
         <v>1</v>
       </c>
+      <c r="W129" s="5">
+        <f t="shared" si="7"/>
+        <v>6027</v>
+      </c>
+      <c r="X129" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99160908193484698</v>
+      </c>
       <c r="Y129" s="1">
         <v>146</v>
       </c>
@@ -6943,6 +7880,14 @@
       <c r="V130">
         <v>1</v>
       </c>
+      <c r="W130" s="5">
+        <f t="shared" si="7"/>
+        <v>6028</v>
+      </c>
+      <c r="X130" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99177360974004602</v>
+      </c>
       <c r="Y130" s="1">
         <v>149</v>
       </c>
@@ -6990,6 +7935,14 @@
       <c r="V131">
         <v>1</v>
       </c>
+      <c r="W131" s="5">
+        <f t="shared" si="7"/>
+        <v>6029</v>
+      </c>
+      <c r="X131" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99193813754524518</v>
+      </c>
       <c r="Y131" s="1">
         <v>164</v>
       </c>
@@ -7037,6 +7990,14 @@
       <c r="V132">
         <v>2</v>
       </c>
+      <c r="W132" s="5">
+        <f t="shared" si="7"/>
+        <v>6031</v>
+      </c>
+      <c r="X132" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99226719315564327</v>
+      </c>
       <c r="Z132">
         <f>SUM(Z13:Z131)</f>
         <v>1270</v>
@@ -7085,6 +8046,14 @@
       <c r="V133">
         <v>3</v>
       </c>
+      <c r="W133" s="5">
+        <f t="shared" si="7"/>
+        <v>6034</v>
+      </c>
+      <c r="X133" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99276077657124051</v>
+      </c>
     </row>
     <row r="134" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K134" s="1">
@@ -7117,6 +8086,14 @@
       <c r="V134">
         <v>3</v>
       </c>
+      <c r="W134" s="5">
+        <f t="shared" si="7"/>
+        <v>6037</v>
+      </c>
+      <c r="X134" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99325435998683775</v>
+      </c>
     </row>
     <row r="135" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K135" s="1">
@@ -7149,6 +8126,14 @@
       <c r="V135">
         <v>3</v>
       </c>
+      <c r="W135" s="5">
+        <f t="shared" si="7"/>
+        <v>6040</v>
+      </c>
+      <c r="X135" s="3">
+        <f t="shared" si="6"/>
+        <v>0.993747943402435</v>
+      </c>
     </row>
     <row r="136" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K136" s="1">
@@ -7181,6 +8166,14 @@
       <c r="V136">
         <v>1</v>
       </c>
+      <c r="W136" s="5">
+        <f t="shared" si="7"/>
+        <v>6041</v>
+      </c>
+      <c r="X136" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99391247120763404</v>
+      </c>
     </row>
     <row r="137" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K137" s="1">
@@ -7213,6 +8206,14 @@
       <c r="V137">
         <v>2</v>
       </c>
+      <c r="W137" s="5">
+        <f t="shared" si="7"/>
+        <v>6043</v>
+      </c>
+      <c r="X137" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99424152681803224</v>
+      </c>
     </row>
     <row r="138" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K138" s="1">
@@ -7245,6 +8246,14 @@
       <c r="V138">
         <v>4</v>
       </c>
+      <c r="W138" s="5">
+        <f t="shared" si="7"/>
+        <v>6047</v>
+      </c>
+      <c r="X138" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99489963803882853</v>
+      </c>
     </row>
     <row r="139" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K139" s="1">
@@ -7277,6 +8286,14 @@
       <c r="V139">
         <v>4</v>
       </c>
+      <c r="W139" s="5">
+        <f t="shared" si="7"/>
+        <v>6051</v>
+      </c>
+      <c r="X139" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99555774925962492</v>
+      </c>
     </row>
     <row r="140" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K140" s="1">
@@ -7309,6 +8326,14 @@
       <c r="V140">
         <v>3</v>
       </c>
+      <c r="W140" s="5">
+        <f t="shared" si="7"/>
+        <v>6054</v>
+      </c>
+      <c r="X140" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99605133267522217</v>
+      </c>
     </row>
     <row r="141" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K141" s="1">
@@ -7341,6 +8366,14 @@
       <c r="V141">
         <v>1</v>
       </c>
+      <c r="W141" s="5">
+        <f t="shared" si="7"/>
+        <v>6055</v>
+      </c>
+      <c r="X141" s="3">
+        <f t="shared" si="6"/>
+        <v>0.99621586048042121</v>
+      </c>
     </row>
     <row r="142" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K142" s="1">
@@ -7373,6 +8406,14 @@
       <c r="V142">
         <v>3</v>
       </c>
+      <c r="W142" s="5">
+        <f t="shared" si="7"/>
+        <v>6058</v>
+      </c>
+      <c r="X142" s="3">
+        <f t="shared" ref="X142:X156" si="8">W142/$V$157</f>
+        <v>0.99670944389601845</v>
+      </c>
     </row>
     <row r="143" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K143" s="1">
@@ -7405,6 +8446,14 @@
       <c r="V143">
         <v>3</v>
       </c>
+      <c r="W143" s="5">
+        <f t="shared" ref="W143:W156" si="9">V143+W142</f>
+        <v>6061</v>
+      </c>
+      <c r="X143" s="3">
+        <f t="shared" si="8"/>
+        <v>0.9972030273116157</v>
+      </c>
     </row>
     <row r="144" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K144" s="1">
@@ -7437,8 +8486,16 @@
       <c r="V144">
         <v>2</v>
       </c>
-    </row>
-    <row r="145" spans="11:22" x14ac:dyDescent="0.2">
+      <c r="W144" s="5">
+        <f t="shared" si="9"/>
+        <v>6063</v>
+      </c>
+      <c r="X144" s="3">
+        <f t="shared" si="8"/>
+        <v>0.99753208292201379</v>
+      </c>
+    </row>
+    <row r="145" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K145" s="1">
         <v>633</v>
       </c>
@@ -7469,8 +8526,16 @@
       <c r="V145">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="11:22" x14ac:dyDescent="0.2">
+      <c r="W145" s="5">
+        <f t="shared" si="9"/>
+        <v>6064</v>
+      </c>
+      <c r="X145" s="3">
+        <f t="shared" si="8"/>
+        <v>0.99769661072721294</v>
+      </c>
+    </row>
+    <row r="146" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K146" s="1">
         <v>634</v>
       </c>
@@ -7501,8 +8566,16 @@
       <c r="V146">
         <v>2</v>
       </c>
-    </row>
-    <row r="147" spans="11:22" x14ac:dyDescent="0.2">
+      <c r="W146" s="5">
+        <f t="shared" si="9"/>
+        <v>6066</v>
+      </c>
+      <c r="X146" s="3">
+        <f t="shared" si="8"/>
+        <v>0.99802566633761103</v>
+      </c>
+    </row>
+    <row r="147" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K147" s="1">
         <v>635</v>
       </c>
@@ -7533,8 +8606,16 @@
       <c r="V147">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="11:22" x14ac:dyDescent="0.2">
+      <c r="W147" s="5">
+        <f t="shared" si="9"/>
+        <v>6067</v>
+      </c>
+      <c r="X147" s="3">
+        <f t="shared" si="8"/>
+        <v>0.99819019414281018</v>
+      </c>
+    </row>
+    <row r="148" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K148" s="1">
         <v>636</v>
       </c>
@@ -7565,8 +8646,16 @@
       <c r="V148">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="11:22" x14ac:dyDescent="0.2">
+      <c r="W148" s="5">
+        <f t="shared" si="9"/>
+        <v>6068</v>
+      </c>
+      <c r="X148" s="3">
+        <f t="shared" si="8"/>
+        <v>0.99835472194800923</v>
+      </c>
+    </row>
+    <row r="149" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K149" s="1">
         <v>637</v>
       </c>
@@ -7597,8 +8686,16 @@
       <c r="V149">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="11:22" x14ac:dyDescent="0.2">
+      <c r="W149" s="5">
+        <f t="shared" si="9"/>
+        <v>6069</v>
+      </c>
+      <c r="X149" s="3">
+        <f t="shared" si="8"/>
+        <v>0.99851924975320827</v>
+      </c>
+    </row>
+    <row r="150" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K150" s="1">
         <v>638</v>
       </c>
@@ -7629,8 +8726,16 @@
       <c r="V150">
         <v>3</v>
       </c>
-    </row>
-    <row r="151" spans="11:22" x14ac:dyDescent="0.2">
+      <c r="W150" s="5">
+        <f t="shared" si="9"/>
+        <v>6072</v>
+      </c>
+      <c r="X150" s="3">
+        <f t="shared" si="8"/>
+        <v>0.99901283316880551</v>
+      </c>
+    </row>
+    <row r="151" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K151" s="1">
         <v>639</v>
       </c>
@@ -7661,8 +8766,16 @@
       <c r="V151">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="11:22" x14ac:dyDescent="0.2">
+      <c r="W151" s="5">
+        <f t="shared" si="9"/>
+        <v>6073</v>
+      </c>
+      <c r="X151" s="3">
+        <f t="shared" si="8"/>
+        <v>0.99917736097400456</v>
+      </c>
+    </row>
+    <row r="152" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K152" s="1">
         <v>641</v>
       </c>
@@ -7693,8 +8806,16 @@
       <c r="V152">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="11:22" x14ac:dyDescent="0.2">
+      <c r="W152" s="5">
+        <f t="shared" si="9"/>
+        <v>6074</v>
+      </c>
+      <c r="X152" s="3">
+        <f t="shared" si="8"/>
+        <v>0.99934188877920371</v>
+      </c>
+    </row>
+    <row r="153" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K153" s="1">
         <v>642</v>
       </c>
@@ -7725,8 +8846,16 @@
       <c r="V153">
         <v>1</v>
       </c>
-    </row>
-    <row r="154" spans="11:22" x14ac:dyDescent="0.2">
+      <c r="W153" s="5">
+        <f t="shared" si="9"/>
+        <v>6075</v>
+      </c>
+      <c r="X153" s="3">
+        <f t="shared" si="8"/>
+        <v>0.99950641658440276</v>
+      </c>
+    </row>
+    <row r="154" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K154" s="1">
         <v>643</v>
       </c>
@@ -7757,8 +8886,16 @@
       <c r="V154">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="11:22" x14ac:dyDescent="0.2">
+      <c r="W154" s="5">
+        <f t="shared" si="9"/>
+        <v>6076</v>
+      </c>
+      <c r="X154" s="3">
+        <f t="shared" si="8"/>
+        <v>0.9996709443896018</v>
+      </c>
+    </row>
+    <row r="155" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K155" s="1">
         <v>644</v>
       </c>
@@ -7789,8 +8926,16 @@
       <c r="V155">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="11:22" x14ac:dyDescent="0.2">
+      <c r="W155" s="5">
+        <f t="shared" si="9"/>
+        <v>6077</v>
+      </c>
+      <c r="X155" s="3">
+        <f t="shared" si="8"/>
+        <v>0.99983547219480096</v>
+      </c>
+    </row>
+    <row r="156" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K156" s="1">
         <v>646</v>
       </c>
@@ -7821,8 +8966,16 @@
       <c r="V156">
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="11:22" x14ac:dyDescent="0.2">
+      <c r="W156" s="5">
+        <f t="shared" si="9"/>
+        <v>6078</v>
+      </c>
+      <c r="X156" s="3">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K157" s="1">
         <v>647</v>
       </c>
@@ -7855,7 +9008,7 @@
         <v>6078</v>
       </c>
     </row>
-    <row r="158" spans="11:22" x14ac:dyDescent="0.2">
+    <row r="158" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K158" s="1">
         <v>648</v>
       </c>
@@ -7872,7 +9025,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="159" spans="11:22" x14ac:dyDescent="0.2">
+    <row r="159" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K159" s="1">
         <v>650</v>
       </c>
@@ -7889,7 +9042,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="11:22" x14ac:dyDescent="0.2">
+    <row r="160" spans="11:24" x14ac:dyDescent="0.2">
       <c r="K160" s="1">
         <v>651</v>
       </c>

</xml_diff>